<commit_message>
#327 Automatisation mapping (#342)
* #327 Ajout des profils d'acces

* Typo mapping

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com> 82a0f298a40d10fcf668ea01514a25bd2def2a38
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice-psychiatric-sector.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice-psychiatric-sector.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-02T15:41:03+00:00</t>
+    <t>2024-04-02T16:06:43+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -341,7 +341,7 @@
 </t>
   </si>
   <si>
-    <t>utilisation</t>
+    <t>secteurPsychiatrique</t>
   </si>
 </sst>
 </file>

</xml_diff>